<commit_message>
fixed mismatching data in health personnel dataset
</commit_message>
<xml_diff>
--- a/data101_data/health_personnel_cleaned.xlsx
+++ b/data101_data/health_personnel_cleaned.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JUPYTER FILES\DATA101\Project\Final Project Dash App\D101_Interactive_Visualization_Project\data101_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA40E4D-A4F3-4034-993A-C31534868710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2CFEBC1-D034-412B-8FAB-383BD686C364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="3396" windowWidth="19140" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -232,9 +232,6 @@
     <t>RIZAL</t>
   </si>
   <si>
-    <t>CITY  OF ISABELA (NOT A PROVINCE)</t>
-  </si>
-  <si>
     <t>ZAMBOANGA DEL NORTE</t>
   </si>
   <si>
@@ -371,6 +368,9 @@
   </si>
   <si>
     <t>NCR, CITY OF MANILA, FIRST DISTRICT (NOT A PROVINCE)</t>
+  </si>
+  <si>
+    <t>CITY OF ISABELA (NOT A PROVINCE)</t>
   </si>
 </sst>
 </file>
@@ -740,8 +740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1448,7 +1448,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C18">
         <v>2947</v>
@@ -2473,7 +2473,7 @@
         <v>21</v>
       </c>
       <c r="B43" t="s">
-        <v>70</v>
+        <v>116</v>
       </c>
       <c r="C43">
         <v>32</v>
@@ -2514,7 +2514,7 @@
         <v>21</v>
       </c>
       <c r="B44" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C44">
         <v>172</v>
@@ -2555,7 +2555,7 @@
         <v>21</v>
       </c>
       <c r="B45" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C45">
         <v>589</v>
@@ -2596,7 +2596,7 @@
         <v>21</v>
       </c>
       <c r="B46" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C46">
         <v>91</v>
@@ -2637,7 +2637,7 @@
         <v>22</v>
       </c>
       <c r="B47" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C47">
         <v>411</v>
@@ -2678,7 +2678,7 @@
         <v>22</v>
       </c>
       <c r="B48" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C48">
         <v>111</v>
@@ -2719,7 +2719,7 @@
         <v>22</v>
       </c>
       <c r="B49" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C49">
         <v>482</v>
@@ -2760,7 +2760,7 @@
         <v>22</v>
       </c>
       <c r="B50" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C50">
         <v>78</v>
@@ -2801,7 +2801,7 @@
         <v>22</v>
       </c>
       <c r="B51" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C51">
         <v>73</v>
@@ -2842,7 +2842,7 @@
         <v>22</v>
       </c>
       <c r="B52" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C52">
         <v>117</v>
@@ -2883,7 +2883,7 @@
         <v>23</v>
       </c>
       <c r="B53" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C53">
         <v>155</v>
@@ -2924,7 +2924,7 @@
         <v>23</v>
       </c>
       <c r="B54" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C54">
         <v>101</v>
@@ -2965,7 +2965,7 @@
         <v>23</v>
       </c>
       <c r="B55" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C55">
         <v>204</v>
@@ -3006,7 +3006,7 @@
         <v>23</v>
       </c>
       <c r="B56" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C56">
         <v>9</v>
@@ -3047,7 +3047,7 @@
         <v>23</v>
       </c>
       <c r="B57" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C57">
         <v>1293</v>
@@ -3088,7 +3088,7 @@
         <v>23</v>
       </c>
       <c r="B58" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C58">
         <v>336</v>
@@ -3129,7 +3129,7 @@
         <v>24</v>
       </c>
       <c r="B59" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C59">
         <v>238</v>
@@ -3170,7 +3170,7 @@
         <v>24</v>
       </c>
       <c r="B60" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C60">
         <v>1467</v>
@@ -3211,7 +3211,7 @@
         <v>24</v>
       </c>
       <c r="B61" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C61">
         <v>205</v>
@@ -3252,7 +3252,7 @@
         <v>24</v>
       </c>
       <c r="B62" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C62">
         <v>8</v>
@@ -3293,7 +3293,7 @@
         <v>25</v>
       </c>
       <c r="B63" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C63">
         <v>25</v>
@@ -3334,7 +3334,7 @@
         <v>25</v>
       </c>
       <c r="B64" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C64">
         <v>68</v>
@@ -3375,7 +3375,7 @@
         <v>25</v>
       </c>
       <c r="B65" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C65">
         <v>691</v>
@@ -3416,7 +3416,7 @@
         <v>25</v>
       </c>
       <c r="B66" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C66">
         <v>69</v>
@@ -3457,7 +3457,7 @@
         <v>25</v>
       </c>
       <c r="B67" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C67">
         <v>50</v>
@@ -3498,7 +3498,7 @@
         <v>25</v>
       </c>
       <c r="B68" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C68">
         <v>82</v>
@@ -3539,7 +3539,7 @@
         <v>26</v>
       </c>
       <c r="B69" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C69">
         <v>265</v>
@@ -3580,7 +3580,7 @@
         <v>26</v>
       </c>
       <c r="B70" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C70">
         <v>22</v>
@@ -3621,7 +3621,7 @@
         <v>26</v>
       </c>
       <c r="B71" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C71">
         <v>185</v>
@@ -3662,7 +3662,7 @@
         <v>26</v>
       </c>
       <c r="B72" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C72">
         <v>161</v>
@@ -3703,7 +3703,7 @@
         <v>26</v>
       </c>
       <c r="B73" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C73">
         <v>533</v>
@@ -3744,7 +3744,7 @@
         <v>27</v>
       </c>
       <c r="B74" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C74">
         <v>87</v>
@@ -3785,7 +3785,7 @@
         <v>27</v>
       </c>
       <c r="B75" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C75">
         <v>285</v>
@@ -3826,7 +3826,7 @@
         <v>27</v>
       </c>
       <c r="B76" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C76">
         <v>922</v>
@@ -3867,7 +3867,7 @@
         <v>27</v>
       </c>
       <c r="B77" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C77">
         <v>42</v>
@@ -3908,7 +3908,7 @@
         <v>27</v>
       </c>
       <c r="B78" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C78">
         <v>84</v>
@@ -3949,7 +3949,7 @@
         <v>28</v>
       </c>
       <c r="B79" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C79">
         <v>284</v>
@@ -3990,7 +3990,7 @@
         <v>28</v>
       </c>
       <c r="B80" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C80">
         <v>111</v>
@@ -4031,7 +4031,7 @@
         <v>28</v>
       </c>
       <c r="B81" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C81">
         <v>22</v>
@@ -4072,7 +4072,7 @@
         <v>28</v>
       </c>
       <c r="B82" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C82">
         <v>365</v>
@@ -4113,7 +4113,7 @@
         <v>28</v>
       </c>
       <c r="B83" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C83">
         <v>144</v>
@@ -4154,7 +4154,7 @@
         <v>29</v>
       </c>
       <c r="B84" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C84">
         <v>158</v>
@@ -4195,7 +4195,7 @@
         <v>29</v>
       </c>
       <c r="B85" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C85">
         <v>61</v>
@@ -4236,7 +4236,7 @@
         <v>29</v>
       </c>
       <c r="B86" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C86">
         <v>16</v>
@@ -4277,7 +4277,7 @@
         <v>29</v>
       </c>
       <c r="B87" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C87">
         <v>91</v>
@@ -4318,7 +4318,7 @@
         <v>29</v>
       </c>
       <c r="B88" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C88">
         <v>137</v>

</xml_diff>